<commit_message>
aproaching the final fix of the lost focus problem by solving the final issue of logging in in headless mode , we just want to confirm not to repeate login each time
</commit_message>
<xml_diff>
--- a/01-01_for_جيانا.xlsx
+++ b/01-01_for_جيانا.xlsx
@@ -26,12 +26,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00FF0000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,8 +52,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,23 +460,53 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="B4" s="1" t="n">
+        <v>12.07</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>oonln-VJU-004647078</t>
+        </is>
+      </c>
+    </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="B5" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>ivon-VJU-004645824</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="1" t="n">
+        <v>70.52</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>alqa-HEB-004624165</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
         <is>
           <t xml:space="preserve">Average = </t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>6.68</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="B8" t="n">
+        <v>19.48</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
         <is>
           <t xml:space="preserve">COD COUNT = </t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="B10" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
The Final version of the GUI programm , fixes the login issue , headless issue and adds a red/green light label , add some beep sounds on fail and success , add killer functions to end subprocesses
</commit_message>
<xml_diff>
--- a/01-01_for_جيانا.xlsx
+++ b/01-01_for_جيانا.xlsx
@@ -26,18 +26,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
-        <bgColor rgb="00FF0000"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -52,9 +46,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -420,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,63 +443,23 @@
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="B3" t="n">
-        <v>6.73</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>WOLRE-JAR-004638630</t>
-        </is>
-      </c>
-    </row>
     <row r="4">
-      <c r="B4" s="1" t="n">
-        <v>12.07</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>oonln-VJU-004647078</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="n">
-        <v>1.48</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>ivon-VJU-004645824</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="1" t="n">
-        <v>70.52</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>alqa-HEB-004624165</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t xml:space="preserve">Average = </t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>19.48</v>
+      <c r="B4" t="n">
+        <v>6.62</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
+    <row r="6">
+      <c r="A6" t="inlineStr">
         <is>
           <t xml:space="preserve">COD COUNT = </t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="B6" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix the autofilling issue in the browsers where credentials are stored, two solutions avalable one of them works , 1- .clear() method on email_field and password_field (doesn't work because the browser fills the field again  ,  2-excute javascript to clear the fields (works perfectly)
</commit_message>
<xml_diff>
--- a/01-01_for_جيانا.xlsx
+++ b/01-01_for_جيانا.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,16 +433,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="B2" t="n">
-        <v>6.62</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>YSKUW-VJU-004622107</t>
-        </is>
-      </c>
-    </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
@@ -450,7 +440,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6.62</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">

</xml_diff>